<commit_message>
Added home + testcase
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TD_HomePage.xlsx
+++ b/src/main/resources/testdata/TD_HomePage.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JavaProjects\Selenium-V1\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C3B483-22A5-4E74-A624-B7BCD44D0A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD27C55B-250E-423D-928E-030AC6CB713A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4425" yWindow="675" windowWidth="16200" windowHeight="9307" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HomePageTitle" sheetId="1" r:id="rId1"/>
     <sheet name="AppDownloadLink" sheetId="2" r:id="rId2"/>
+    <sheet name="ContactEmailAddress" sheetId="3" r:id="rId3"/>
+    <sheet name="FooterLinks" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
   <si>
     <t>Value</t>
   </si>
@@ -34,23 +36,149 @@
     <t>Key</t>
   </si>
   <si>
-    <t>pageTitle</t>
-  </si>
-  <si>
     <t>Shuru App</t>
   </si>
   <si>
-    <t>DownlaodLink</t>
-  </si>
-  <si>
     <t>https://play.google.com/store/apps/details?id=com.shuru.nearme</t>
+  </si>
+  <si>
+    <t>Page Title</t>
+  </si>
+  <si>
+    <t>Downlaod Link</t>
+  </si>
+  <si>
+    <t>Email Address</t>
+  </si>
+  <si>
+    <t>info@shuru.co.in</t>
+  </si>
+  <si>
+    <t>Link Text</t>
+  </si>
+  <si>
+    <t>Link Route</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Contact Us</t>
+  </si>
+  <si>
+    <t>Terms and Conditions</t>
+  </si>
+  <si>
+    <t>Privacy Policy</t>
+  </si>
+  <si>
+    <t>Team and Career</t>
+  </si>
+  <si>
+    <t>Blogs</t>
+  </si>
+  <si>
+    <t>Refund and Cancellation Policy</t>
+  </si>
+  <si>
+    <t>About Us</t>
+  </si>
+  <si>
+    <t>News and Politics</t>
+  </si>
+  <si>
+    <t>News</t>
+  </si>
+  <si>
+    <t>Latest News</t>
+  </si>
+  <si>
+    <t>Elections</t>
+  </si>
+  <si>
+    <t>Politics</t>
+  </si>
+  <si>
+    <t>Latest Political News</t>
+  </si>
+  <si>
+    <t>Astrology</t>
+  </si>
+  <si>
+    <t>Horoscope in Hindi</t>
+  </si>
+  <si>
+    <t>Horoscope in English</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>Viral</t>
+  </si>
+  <si>
+    <t>Mandi</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>/contact-us</t>
+  </si>
+  <si>
+    <t>/terms-and-conditions</t>
+  </si>
+  <si>
+    <t>/privacy-policy</t>
+  </si>
+  <si>
+    <t>/blogs</t>
+  </si>
+  <si>
+    <t>/news</t>
+  </si>
+  <si>
+    <t>/latest-political-news</t>
+  </si>
+  <si>
+    <t>/astrology</t>
+  </si>
+  <si>
+    <t>/services</t>
+  </si>
+  <si>
+    <t>/mandi</t>
+  </si>
+  <si>
+    <t>/career</t>
+  </si>
+  <si>
+    <t>/pricing</t>
+  </si>
+  <si>
+    <t>/category/news</t>
+  </si>
+  <si>
+    <t>/election</t>
+  </si>
+  <si>
+    <t>/category/politics</t>
+  </si>
+  <si>
+    <t>/astrology/horoscope-today-hindi</t>
+  </si>
+  <si>
+    <t>/astrology/horoscope-today-english</t>
+  </si>
+  <si>
+    <t>/category/viral</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +202,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -96,10 +229,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -384,7 +518,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" activeCellId="1" sqref="A1 B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -403,10 +537,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -419,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939ABB28-2C9F-4A7D-B77F-EC9CA31CF436}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -439,10 +573,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -451,4 +585,261 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79972767-DB41-411B-823E-4BC0D81E452F}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="13.06640625" customWidth="1"/>
+    <col min="2" max="2" width="32.3984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{DD885E7B-1E60-4975-B684-9E9D1D1B0C52}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE5A53F7-8536-4259-BE2E-85A44B0F3D2E}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="24.265625" customWidth="1"/>
+    <col min="2" max="2" width="29.53125" customWidth="1"/>
+    <col min="3" max="3" width="36.46484375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added Jackson for json operations
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TD_HomePage.xlsx
+++ b/src/main/resources/testdata/TD_HomePage.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JavaProjects\Selenium-V1\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DCBFF9-B02F-4FA6-A8D6-E636467DDD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED140C8-1051-49EE-B4A1-B5C2DBAC9E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HomePageTitle" sheetId="1" r:id="rId1"/>
     <sheet name="AppDownloadLink" sheetId="2" r:id="rId2"/>
     <sheet name="ContactEmailAddress" sheetId="3" r:id="rId3"/>
     <sheet name="FooterLinks" sheetId="4" r:id="rId4"/>
+    <sheet name="SocialMedia" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
   <si>
     <t>Value</t>
   </si>
@@ -175,6 +176,39 @@
   </si>
   <si>
     <t>/services</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Twitter</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>YouTube</t>
+  </si>
+  <si>
+    <t>LinkedIn</t>
+  </si>
+  <si>
+    <t>Instagram</t>
+  </si>
+  <si>
+    <t>https://twitter.com/Public_Shuru</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@Shuru-App</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/company/shuruindia/</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/shuru.app/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/ShuruAppIndia</t>
   </si>
 </sst>
 </file>
@@ -521,7 +555,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -632,7 +666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE5A53F7-8536-4259-BE2E-85A44B0F3D2E}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -899,4 +933,95 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D25B57F5-6DE4-4D76-9B2D-76E46C9DA3B4}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="75.46484375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{F6657141-53EE-4B95-A935-1A6A605F0D58}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{87DD9E12-BC69-4701-9A96-AF36B31EB1B3}"/>
+    <hyperlink ref="C6" r:id="rId3" xr:uid="{B0D356BE-0270-496E-94A9-62C5DEE591A1}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{BE85A1CE-1D3C-4A29-8887-B6521797EE9A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed soft assertion issue
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TD_HomePage.xlsx
+++ b/src/main/resources/testdata/TD_HomePage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JavaProjects\Selenium-V1\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD27C55B-250E-423D-928E-030AC6CB713A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DCBFF9-B02F-4FA6-A8D6-E636467DDD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>Value</t>
   </si>
@@ -129,49 +129,52 @@
     <t>/terms-and-conditions</t>
   </si>
   <si>
+    <t>/blogs</t>
+  </si>
+  <si>
+    <t>/news</t>
+  </si>
+  <si>
+    <t>/latest-political-news</t>
+  </si>
+  <si>
+    <t>/astrology</t>
+  </si>
+  <si>
+    <t>/mandi</t>
+  </si>
+  <si>
+    <t>/pricing</t>
+  </si>
+  <si>
+    <t>/category/news</t>
+  </si>
+  <si>
+    <t>/election</t>
+  </si>
+  <si>
+    <t>/category/politics</t>
+  </si>
+  <si>
+    <t>/astrology/horoscope-today-hindi</t>
+  </si>
+  <si>
+    <t>/astrology/horoscope-today-english</t>
+  </si>
+  <si>
+    <t>/category/viral</t>
+  </si>
+  <si>
     <t>/privacy-policy</t>
   </si>
   <si>
-    <t>/blogs</t>
-  </si>
-  <si>
-    <t>/news</t>
-  </si>
-  <si>
-    <t>/latest-political-news</t>
-  </si>
-  <si>
-    <t>/astrology</t>
+    <t>/career</t>
+  </si>
+  <si>
+    <t>Index</t>
   </si>
   <si>
     <t>/services</t>
-  </si>
-  <si>
-    <t>/mandi</t>
-  </si>
-  <si>
-    <t>/career</t>
-  </si>
-  <si>
-    <t>/pricing</t>
-  </si>
-  <si>
-    <t>/category/news</t>
-  </si>
-  <si>
-    <t>/election</t>
-  </si>
-  <si>
-    <t>/category/politics</t>
-  </si>
-  <si>
-    <t>/astrology/horoscope-today-hindi</t>
-  </si>
-  <si>
-    <t>/astrology/horoscope-today-english</t>
-  </si>
-  <si>
-    <t>/category/viral</t>
   </si>
 </sst>
 </file>
@@ -627,215 +630,269 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE5A53F7-8536-4259-BE2E-85A44B0F3D2E}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.265625" customWidth="1"/>
-    <col min="2" max="2" width="29.53125" customWidth="1"/>
-    <col min="3" max="3" width="36.46484375" customWidth="1"/>
+    <col min="2" max="2" width="24.265625" customWidth="1"/>
+    <col min="3" max="3" width="29.53125" customWidth="1"/>
+    <col min="4" max="4" width="36.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>1.2</v>
+      </c>
+      <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>1.3</v>
+      </c>
+      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>1.4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>1.5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>1.6</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>2.1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>2.4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>2.5</v>
+      </c>
+      <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>3.1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>3.2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>3.3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>3.4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>3.5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>3.6</v>
+      </c>
+      <c r="B18" t="s">
         <v>30</v>
       </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added services page testcases
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TD_HomePage.xlsx
+++ b/src/main/resources/testdata/TD_HomePage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JavaProjects\Selenium-V1\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED140C8-1051-49EE-B4A1-B5C2DBAC9E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B290DEC1-FD4D-476C-8F0F-BBC75994D5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HomePageTitle" sheetId="1" r:id="rId1"/>
@@ -136,9 +136,6 @@
     <t>/news</t>
   </si>
   <si>
-    <t>/latest-political-news</t>
-  </si>
-  <si>
     <t>/astrology</t>
   </si>
   <si>
@@ -209,6 +206,9 @@
   </si>
   <si>
     <t>https://www.facebook.com/ShuruAppIndia</t>
+  </si>
+  <si>
+    <t>/latest-news</t>
   </si>
 </sst>
 </file>
@@ -666,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE5A53F7-8536-4259-BE2E-85A44B0F3D2E}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -679,7 +679,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>10</v>
@@ -730,7 +730,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
@@ -744,7 +744,7 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
@@ -772,7 +772,7 @@
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
@@ -800,7 +800,7 @@
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
@@ -814,7 +814,7 @@
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
@@ -828,7 +828,7 @@
         <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
@@ -842,7 +842,7 @@
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
@@ -856,7 +856,7 @@
         <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
@@ -870,7 +870,7 @@
         <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
@@ -884,7 +884,7 @@
         <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
@@ -898,7 +898,7 @@
         <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
@@ -912,7 +912,7 @@
         <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
@@ -926,7 +926,7 @@
         <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -939,7 +939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D25B57F5-6DE4-4D76-9B2D-76E46C9DA3B4}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -951,13 +951,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -965,10 +965,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -976,10 +976,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -987,10 +987,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
@@ -998,10 +998,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
@@ -1009,10 +1009,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
addes services testcases and updated master.xml
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TD_HomePage.xlsx
+++ b/src/main/resources/testdata/TD_HomePage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JavaProjects\Selenium-V1\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED140C8-1051-49EE-B4A1-B5C2DBAC9E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B290DEC1-FD4D-476C-8F0F-BBC75994D5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HomePageTitle" sheetId="1" r:id="rId1"/>
@@ -136,9 +136,6 @@
     <t>/news</t>
   </si>
   <si>
-    <t>/latest-political-news</t>
-  </si>
-  <si>
     <t>/astrology</t>
   </si>
   <si>
@@ -209,6 +206,9 @@
   </si>
   <si>
     <t>https://www.facebook.com/ShuruAppIndia</t>
+  </si>
+  <si>
+    <t>/latest-news</t>
   </si>
 </sst>
 </file>
@@ -666,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE5A53F7-8536-4259-BE2E-85A44B0F3D2E}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -679,7 +679,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>10</v>
@@ -730,7 +730,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
@@ -744,7 +744,7 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
@@ -772,7 +772,7 @@
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
@@ -800,7 +800,7 @@
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
@@ -814,7 +814,7 @@
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
@@ -828,7 +828,7 @@
         <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
@@ -842,7 +842,7 @@
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
@@ -856,7 +856,7 @@
         <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
@@ -870,7 +870,7 @@
         <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
@@ -884,7 +884,7 @@
         <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
@@ -898,7 +898,7 @@
         <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
@@ -912,7 +912,7 @@
         <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
@@ -926,7 +926,7 @@
         <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -939,7 +939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D25B57F5-6DE4-4D76-9B2D-76E46C9DA3B4}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -951,13 +951,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -965,10 +965,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -976,10 +976,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -987,10 +987,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
@@ -998,10 +998,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
@@ -1009,10 +1009,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated new footer links in home excel
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TD_HomePage.xlsx
+++ b/src/main/resources/testdata/TD_HomePage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JavaProjects\Selenium-V1\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B290DEC1-FD4D-476C-8F0F-BBC75994D5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC945AF-A9AD-490A-950F-04DD70FF0D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="278">
   <si>
     <t>Value</t>
   </si>
@@ -85,21 +85,12 @@
     <t>About Us</t>
   </si>
   <si>
-    <t>News and Politics</t>
-  </si>
-  <si>
     <t>News</t>
   </si>
   <si>
-    <t>Latest News</t>
-  </si>
-  <si>
     <t>Elections</t>
   </si>
   <si>
-    <t>Politics</t>
-  </si>
-  <si>
     <t>Latest Political News</t>
   </si>
   <si>
@@ -115,66 +106,9 @@
     <t>Services</t>
   </si>
   <si>
-    <t>Viral</t>
-  </si>
-  <si>
-    <t>Mandi</t>
-  </si>
-  <si>
-    <t>Categories</t>
-  </si>
-  <si>
-    <t>/contact-us</t>
-  </si>
-  <si>
-    <t>/terms-and-conditions</t>
-  </si>
-  <si>
-    <t>/blogs</t>
-  </si>
-  <si>
-    <t>/news</t>
-  </si>
-  <si>
-    <t>/astrology</t>
-  </si>
-  <si>
-    <t>/mandi</t>
-  </si>
-  <si>
-    <t>/pricing</t>
-  </si>
-  <si>
-    <t>/category/news</t>
-  </si>
-  <si>
-    <t>/election</t>
-  </si>
-  <si>
-    <t>/category/politics</t>
-  </si>
-  <si>
-    <t>/astrology/horoscope-today-hindi</t>
-  </si>
-  <si>
-    <t>/astrology/horoscope-today-english</t>
-  </si>
-  <si>
-    <t>/category/viral</t>
-  </si>
-  <si>
-    <t>/privacy-policy</t>
-  </si>
-  <si>
-    <t>/career</t>
-  </si>
-  <si>
     <t>Index</t>
   </si>
   <si>
-    <t>/services</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
@@ -208,14 +142,734 @@
     <t>https://www.facebook.com/ShuruAppIndia</t>
   </si>
   <si>
-    <t>/latest-news</t>
+    <t>Top Electrician Services</t>
+  </si>
+  <si>
+    <t>Top Carpenter Services</t>
+  </si>
+  <si>
+    <t>Top Astrologer Services</t>
+  </si>
+  <si>
+    <t>Top Plumber Services</t>
+  </si>
+  <si>
+    <t>Mandi Services</t>
+  </si>
+  <si>
+    <t>Daily Horoscope</t>
+  </si>
+  <si>
+    <t>Astrology and Panchang</t>
+  </si>
+  <si>
+    <t>Quick Links</t>
+  </si>
+  <si>
+    <t>Electrician in Jabalpur</t>
+  </si>
+  <si>
+    <t>Electrician in Raipur</t>
+  </si>
+  <si>
+    <t>Electrician in Surat</t>
+  </si>
+  <si>
+    <t>Electrician in Kanpur</t>
+  </si>
+  <si>
+    <t>Electrician in Vadodara</t>
+  </si>
+  <si>
+    <t>Electrician in Nagpur</t>
+  </si>
+  <si>
+    <t>Electrician in Nashik</t>
+  </si>
+  <si>
+    <t>Electrician in Rajkot</t>
+  </si>
+  <si>
+    <t>Electrician in Jaipur</t>
+  </si>
+  <si>
+    <t>Electrician in Indore</t>
+  </si>
+  <si>
+    <t>Electrician in Pune</t>
+  </si>
+  <si>
+    <t>Electrician in Hyderabad</t>
+  </si>
+  <si>
+    <t>Carpenter in Jabalpur</t>
+  </si>
+  <si>
+    <t>Carpenter in Raipur</t>
+  </si>
+  <si>
+    <t>Carpenter in Surat</t>
+  </si>
+  <si>
+    <t>Carpenter in Kanpur</t>
+  </si>
+  <si>
+    <t>Carpenter in Vadodara</t>
+  </si>
+  <si>
+    <t>Carpenter in Nagpur</t>
+  </si>
+  <si>
+    <t>Carpenter in Nashik</t>
+  </si>
+  <si>
+    <t>Carpenter in Rajkot</t>
+  </si>
+  <si>
+    <t>Carpenter in Jaipur</t>
+  </si>
+  <si>
+    <t>Carpenter in Indore</t>
+  </si>
+  <si>
+    <t>Carpenter in Pune</t>
+  </si>
+  <si>
+    <t>Carpenter in Hyderabad</t>
+  </si>
+  <si>
+    <t>Astrologer in Jabalpur</t>
+  </si>
+  <si>
+    <t>Astrologer in Raipur</t>
+  </si>
+  <si>
+    <t>Astrologer in Surat</t>
+  </si>
+  <si>
+    <t>Astrologer in Kanpur</t>
+  </si>
+  <si>
+    <t>Astrologer in Vadodara</t>
+  </si>
+  <si>
+    <t>Astrologer in Nagpur</t>
+  </si>
+  <si>
+    <t>Astrologer in Nashik</t>
+  </si>
+  <si>
+    <t>Astrologer in Rajkot</t>
+  </si>
+  <si>
+    <t>Astrologer in Jaipur</t>
+  </si>
+  <si>
+    <t>Astrologer in Pune</t>
+  </si>
+  <si>
+    <t>Astrologer in Hyderabad</t>
+  </si>
+  <si>
+    <t>Plumber in Jabalpur</t>
+  </si>
+  <si>
+    <t>Plumber in Raipur</t>
+  </si>
+  <si>
+    <t>Plumber in Surat</t>
+  </si>
+  <si>
+    <t>Plumber in Kanpur</t>
+  </si>
+  <si>
+    <t>Plumber in Vadodara</t>
+  </si>
+  <si>
+    <t>Plumber in Nagpur</t>
+  </si>
+  <si>
+    <t>Plumber in Nashik</t>
+  </si>
+  <si>
+    <t>Plumber in Rajkot</t>
+  </si>
+  <si>
+    <t>Plumber in Jaipur</t>
+  </si>
+  <si>
+    <t>Plumber in Indore</t>
+  </si>
+  <si>
+    <t>Plumber in Pune</t>
+  </si>
+  <si>
+    <t>Plumber in Hyderabad</t>
+  </si>
+  <si>
+    <t>Bihar</t>
+  </si>
+  <si>
+    <t>Chattisgarh</t>
+  </si>
+  <si>
+    <t>Madhya Pradesh</t>
+  </si>
+  <si>
+    <t>Maharashtra</t>
+  </si>
+  <si>
+    <t>Nct Of Delhi</t>
+  </si>
+  <si>
+    <t>Karnataka</t>
+  </si>
+  <si>
+    <t>Goa</t>
+  </si>
+  <si>
+    <t>Pondicherry</t>
+  </si>
+  <si>
+    <t>Kerala</t>
+  </si>
+  <si>
+    <t>Odisha</t>
+  </si>
+  <si>
+    <t>Andaman And Nicobar</t>
+  </si>
+  <si>
+    <t>Gujarat</t>
+  </si>
+  <si>
+    <t>Uttar Pradesh</t>
+  </si>
+  <si>
+    <t>Meghalaya</t>
+  </si>
+  <si>
+    <t>Rajasthan</t>
+  </si>
+  <si>
+    <t>Uttrakhand</t>
+  </si>
+  <si>
+    <t>Manipur</t>
+  </si>
+  <si>
+    <t>Andhra Pradesh</t>
+  </si>
+  <si>
+    <t>Punjab</t>
+  </si>
+  <si>
+    <t>Tamil Nadu</t>
+  </si>
+  <si>
+    <t>Assam</t>
+  </si>
+  <si>
+    <t>Jammu And Kashmir</t>
+  </si>
+  <si>
+    <t>Telangana</t>
+  </si>
+  <si>
+    <t>Tripura</t>
+  </si>
+  <si>
+    <t>Chandigarh</t>
+  </si>
+  <si>
+    <t>Nagaland</t>
+  </si>
+  <si>
+    <t>West Bengal</t>
+  </si>
+  <si>
+    <t>Haryana</t>
+  </si>
+  <si>
+    <t>Himachal Pradesh</t>
+  </si>
+  <si>
+    <t>Horoscope in Assamese</t>
+  </si>
+  <si>
+    <t>Horoscope in Bengali</t>
+  </si>
+  <si>
+    <t>Horoscope in Gujarati</t>
+  </si>
+  <si>
+    <t>Horoscope in Kannada</t>
+  </si>
+  <si>
+    <t>Horoscope in Malayalam</t>
+  </si>
+  <si>
+    <t>Horoscope in Marathi</t>
+  </si>
+  <si>
+    <t>Horoscope in Odia</t>
+  </si>
+  <si>
+    <t>Horoscope in Punjabi</t>
+  </si>
+  <si>
+    <t>Horoscope in Tamil</t>
+  </si>
+  <si>
+    <t>Horoscope in Telugu</t>
+  </si>
+  <si>
+    <t>Aries</t>
+  </si>
+  <si>
+    <t>Taurus</t>
+  </si>
+  <si>
+    <t>Gemini</t>
+  </si>
+  <si>
+    <t>Cancer</t>
+  </si>
+  <si>
+    <t>Leo</t>
+  </si>
+  <si>
+    <t>Virgo</t>
+  </si>
+  <si>
+    <t>Libra</t>
+  </si>
+  <si>
+    <t>Scorpio</t>
+  </si>
+  <si>
+    <t>Sagittarius</t>
+  </si>
+  <si>
+    <t>Capricorn</t>
+  </si>
+  <si>
+    <t>Aquarius</t>
+  </si>
+  <si>
+    <t>Pisces</t>
+  </si>
+  <si>
+    <t>Panchang in English</t>
+  </si>
+  <si>
+    <t>Panchang in Hindi</t>
+  </si>
+  <si>
+    <t>Panchang in Gujarati</t>
+  </si>
+  <si>
+    <t>Panchang in Bangla</t>
+  </si>
+  <si>
+    <t>Panchang in Kannada</t>
+  </si>
+  <si>
+    <t>Panchang in Malayalam</t>
+  </si>
+  <si>
+    <t>Panchang in Marathi</t>
+  </si>
+  <si>
+    <t>Panchang in Odia</t>
+  </si>
+  <si>
+    <t>Panchang in Punjabi</t>
+  </si>
+  <si>
+    <t>Panchang in Tamil</t>
+  </si>
+  <si>
+    <t>Panchang in Telugu</t>
+  </si>
+  <si>
+    <t>Panchang in Assamese</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-electrician-in-jabalpur</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-electrician-in-raipur</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-electrician-in-surat</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-electrician-in-kanpur</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-electrician-in-vadodara</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-electrician-in-nagpur</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-electrician-in-nashik</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-electrician-in-rajkot</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-electrician-in-jaipur</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-electrician-in-indore</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-electrician-in-pune</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-electrician-in-hyderabad</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-carpenter-in-jabalpur</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-carpenter-in-raipur</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-carpenter-in-surat</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-carpenter-in-kanpur</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-carpenter-in-vadodara</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-carpenter-in-nagpur</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-carpenter-in-nashik</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-carpenter-in-rajkot</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-carpenter-in-jaipur</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-carpenter-in-indore</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-carpenter-in-pune</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-carpenter-in-hyderabad</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-astrologer-in-jabalpur</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-astrologer-in-raipur</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-astrologer-in-surat</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-astrologer-in-kanpur</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-astrologer-in-vadodara</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-astrologer-in-nagpur</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-astrologer-in-nashik</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-astrologer-in-rajkot</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-astrologer-in-jaipur</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-astrologer-in-pune</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-astrologer-in-hyderabad</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-plumber-in-jabalpur</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-plumber-in-raipur</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-plumber-in-surat</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-plumber-in-kanpur</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-plumber-in-vadodara</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-plumber-in-nagpur</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-plumber-in-nashik</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-plumber-in-rajkot</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-plumber-in-jaipur</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-plumber-in-indore</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-plumber-in-pune</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services/top-10-plumber-in-hyderabad</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/bihar</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/chattisgarh</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/madhya-pradesh</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/maharashtra</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/nct-of-delhi</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/karnataka</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/goa</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/pondicherry</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/kerala</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/odisha</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/andaman-and-nicobar</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/gujarat</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/uttar-pradesh</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/meghalaya</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/rajasthan</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/uttrakhand</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/manipur</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/andhra-pradesh</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/punjab</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/tamil-nadu</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/assam</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/jammu-and-kashmir</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/telangana</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/tripura</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/chandigarh</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/nagaland</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/west-bengal</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/haryana</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/mandi-bhav/himachal-pradesh</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/horoscope-today-hindi</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/horoscope-today-english</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/horoscope-today-assamese</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/horoscope-today-bangla</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/horoscope-today-gujarati</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/horoscope-today-kannada</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/horoscope-today-malayalam</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/horoscope-today-marathi</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/horoscope-today-odia</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/horoscope-today-punjabi</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/horoscope-today-tamil</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/horoscope-today-telugu</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/aries-horoscope-today-english</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/taurus-horoscope-today-english</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/gemini-horoscope-today-english</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/cancer-horoscope-today-english</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/leo-horoscope-today-english</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/virgo-horoscope-today-english</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/libra-horoscope-today-english</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/scorpio-horoscope-today-english</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/sagittarius-horoscope-today-english</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/capricorn-horoscope-today-english</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/aquarius-horoscope-today-english</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/pisces-horoscope-today-english</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/panchang-today-English</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/panchang-today-Hindi</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/panchang-today-Gujarati</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/panchang-today-Bangla</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/panchang-today-Kannada</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/panchang-today-Malayalam</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/panchang-today-Marathi</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/panchang-today-Odia</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/panchang-today-Punjabi</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/panchang-today-Tamil</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/panchang-today-Telugu</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/astrology/panchang-today-Assamese</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/news</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/services</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/election</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/latest-news</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/blogs</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/contact-us</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/terms-and-conditions</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/privacy-policy</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/career</t>
+  </si>
+  <si>
+    <t>https://shuru.co.in/pricing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,11 +893,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -266,11 +915,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -664,22 +1312,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE5A53F7-8536-4259-BE2E-85A44B0F3D2E}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="F123" sqref="F123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="24.265625" customWidth="1"/>
     <col min="3" max="3" width="29.53125" customWidth="1"/>
-    <col min="4" max="4" width="36.1328125" customWidth="1"/>
+    <col min="4" max="4" width="63.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>10</v>
@@ -696,13 +1344,13 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>31</v>
+        <v>45</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
@@ -710,13 +1358,13 @@
         <v>1.2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
@@ -724,13 +1372,13 @@
         <v>1.3</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
@@ -738,13 +1386,13 @@
         <v>1.4</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
@@ -752,13 +1400,13 @@
         <v>1.5</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
@@ -766,172 +1414,1673 @@
         <v>1.6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>2.1</v>
+        <v>1.7</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>2.2000000000000002</v>
+        <v>1.8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>2.2999999999999998</v>
+        <v>1.9</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11">
-        <v>2.4</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12">
-        <v>2.5</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13">
-        <v>3.1</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14">
-        <v>3.2</v>
+        <v>2.1</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15">
-        <v>3.3</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16">
-        <v>3.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>3.5</v>
+        <v>2.4</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18">
+        <v>2.5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>2.6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>2.7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>2.8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>2.9</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>2.1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>2.11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>2.12</v>
+      </c>
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>3.1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>3.2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>3.3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>3.4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>3.5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31">
         <v>3.6</v>
       </c>
-      <c r="B18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" t="s">
-        <v>36</v>
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>3.7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" t="s">
+        <v>75</v>
+      </c>
+      <c r="D32" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>3.8</v>
+      </c>
+      <c r="B33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>3.9</v>
+      </c>
+      <c r="B34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>3.1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>3.11</v>
+      </c>
+      <c r="B36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" t="s">
+        <v>79</v>
+      </c>
+      <c r="D36" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>4.2</v>
+      </c>
+      <c r="B38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>4.3</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B40" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>4.5</v>
+      </c>
+      <c r="B41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="B42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" t="s">
+        <v>85</v>
+      </c>
+      <c r="D42" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>4.7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" t="s">
+        <v>86</v>
+      </c>
+      <c r="D43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>4.8</v>
+      </c>
+      <c r="B44" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" t="s">
+        <v>87</v>
+      </c>
+      <c r="D44" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" t="s">
+        <v>88</v>
+      </c>
+      <c r="D45" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B46" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46" t="s">
+        <v>89</v>
+      </c>
+      <c r="D46" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="B47" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>4.12</v>
+      </c>
+      <c r="B48" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B49" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" t="s">
+        <v>92</v>
+      </c>
+      <c r="D49" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>5.2</v>
+      </c>
+      <c r="B50" t="s">
+        <v>41</v>
+      </c>
+      <c r="C50" t="s">
+        <v>93</v>
+      </c>
+      <c r="D50" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>5.3</v>
+      </c>
+      <c r="B51" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" t="s">
+        <v>94</v>
+      </c>
+      <c r="D51" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>5.4</v>
+      </c>
+      <c r="B52" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52" t="s">
+        <v>95</v>
+      </c>
+      <c r="D52" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>5.5</v>
+      </c>
+      <c r="B53" t="s">
+        <v>41</v>
+      </c>
+      <c r="C53" t="s">
+        <v>96</v>
+      </c>
+      <c r="D53" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>5.6</v>
+      </c>
+      <c r="B54" t="s">
+        <v>41</v>
+      </c>
+      <c r="C54" t="s">
+        <v>97</v>
+      </c>
+      <c r="D54" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>5.7</v>
+      </c>
+      <c r="B55" t="s">
+        <v>41</v>
+      </c>
+      <c r="C55" t="s">
+        <v>98</v>
+      </c>
+      <c r="D55" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>5.8</v>
+      </c>
+      <c r="B56" t="s">
+        <v>41</v>
+      </c>
+      <c r="C56" t="s">
+        <v>99</v>
+      </c>
+      <c r="D56" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>5.9</v>
+      </c>
+      <c r="B57" t="s">
+        <v>41</v>
+      </c>
+      <c r="C57" t="s">
+        <v>100</v>
+      </c>
+      <c r="D57" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A58">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B58" t="s">
+        <v>41</v>
+      </c>
+      <c r="C58" t="s">
+        <v>101</v>
+      </c>
+      <c r="D58" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="B59" t="s">
+        <v>41</v>
+      </c>
+      <c r="C59" t="s">
+        <v>102</v>
+      </c>
+      <c r="D59" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>5.12</v>
+      </c>
+      <c r="B60" t="s">
+        <v>41</v>
+      </c>
+      <c r="C60" t="s">
+        <v>103</v>
+      </c>
+      <c r="D60" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A61">
+        <v>5.13</v>
+      </c>
+      <c r="B61" t="s">
+        <v>41</v>
+      </c>
+      <c r="C61" t="s">
+        <v>104</v>
+      </c>
+      <c r="D61" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A62">
+        <v>5.14</v>
+      </c>
+      <c r="B62" t="s">
+        <v>41</v>
+      </c>
+      <c r="C62" t="s">
+        <v>105</v>
+      </c>
+      <c r="D62" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>5.15</v>
+      </c>
+      <c r="B63" t="s">
+        <v>41</v>
+      </c>
+      <c r="C63" t="s">
+        <v>106</v>
+      </c>
+      <c r="D63" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>5.16</v>
+      </c>
+      <c r="B64" t="s">
+        <v>41</v>
+      </c>
+      <c r="C64" t="s">
+        <v>107</v>
+      </c>
+      <c r="D64" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>5.17</v>
+      </c>
+      <c r="B65" t="s">
+        <v>41</v>
+      </c>
+      <c r="C65" t="s">
+        <v>108</v>
+      </c>
+      <c r="D65" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A66">
+        <v>5.18</v>
+      </c>
+      <c r="B66" t="s">
+        <v>41</v>
+      </c>
+      <c r="C66" t="s">
+        <v>109</v>
+      </c>
+      <c r="D66" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A67">
+        <v>5.19</v>
+      </c>
+      <c r="B67" t="s">
+        <v>41</v>
+      </c>
+      <c r="C67" t="s">
+        <v>110</v>
+      </c>
+      <c r="D67" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A68">
+        <v>5.2</v>
+      </c>
+      <c r="B68" t="s">
+        <v>41</v>
+      </c>
+      <c r="C68" t="s">
+        <v>101</v>
+      </c>
+      <c r="D68" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A69">
+        <v>5.21</v>
+      </c>
+      <c r="B69" t="s">
+        <v>41</v>
+      </c>
+      <c r="C69" t="s">
+        <v>111</v>
+      </c>
+      <c r="D69" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A70">
+        <v>5.22</v>
+      </c>
+      <c r="B70" t="s">
+        <v>41</v>
+      </c>
+      <c r="C70" t="s">
+        <v>112</v>
+      </c>
+      <c r="D70" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A71">
+        <v>5.23</v>
+      </c>
+      <c r="B71" t="s">
+        <v>41</v>
+      </c>
+      <c r="C71" t="s">
+        <v>113</v>
+      </c>
+      <c r="D71" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A72">
+        <v>5.24</v>
+      </c>
+      <c r="B72" t="s">
+        <v>41</v>
+      </c>
+      <c r="C72" t="s">
+        <v>114</v>
+      </c>
+      <c r="D72" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A73">
+        <v>5.25</v>
+      </c>
+      <c r="B73" t="s">
+        <v>41</v>
+      </c>
+      <c r="C73" t="s">
+        <v>115</v>
+      </c>
+      <c r="D73" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A74">
+        <v>5.26</v>
+      </c>
+      <c r="B74" t="s">
+        <v>41</v>
+      </c>
+      <c r="C74" t="s">
+        <v>116</v>
+      </c>
+      <c r="D74" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A75">
+        <v>5.27</v>
+      </c>
+      <c r="B75" t="s">
+        <v>41</v>
+      </c>
+      <c r="C75" t="s">
+        <v>117</v>
+      </c>
+      <c r="D75" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A76">
+        <v>5.28</v>
+      </c>
+      <c r="B76" t="s">
+        <v>41</v>
+      </c>
+      <c r="C76" t="s">
+        <v>118</v>
+      </c>
+      <c r="D76" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A77">
+        <v>5.29</v>
+      </c>
+      <c r="B77" t="s">
+        <v>41</v>
+      </c>
+      <c r="C77" t="s">
+        <v>119</v>
+      </c>
+      <c r="D77" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A78">
+        <v>5.3</v>
+      </c>
+      <c r="B78" t="s">
+        <v>41</v>
+      </c>
+      <c r="C78" t="s">
+        <v>120</v>
+      </c>
+      <c r="D78" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A79">
+        <v>6.1</v>
+      </c>
+      <c r="B79" t="s">
+        <v>42</v>
+      </c>
+      <c r="C79" t="s">
+        <v>22</v>
+      </c>
+      <c r="D79" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A80">
+        <v>6.2</v>
+      </c>
+      <c r="B80" t="s">
+        <v>42</v>
+      </c>
+      <c r="C80" t="s">
+        <v>23</v>
+      </c>
+      <c r="D80" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A81">
+        <v>6.3</v>
+      </c>
+      <c r="B81" t="s">
+        <v>42</v>
+      </c>
+      <c r="C81" t="s">
+        <v>121</v>
+      </c>
+      <c r="D81" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A82">
+        <v>6.4</v>
+      </c>
+      <c r="B82" t="s">
+        <v>42</v>
+      </c>
+      <c r="C82" t="s">
+        <v>122</v>
+      </c>
+      <c r="D82" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A83">
+        <v>6.5</v>
+      </c>
+      <c r="B83" t="s">
+        <v>42</v>
+      </c>
+      <c r="C83" t="s">
+        <v>123</v>
+      </c>
+      <c r="D83" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A84">
+        <v>6.6</v>
+      </c>
+      <c r="B84" t="s">
+        <v>42</v>
+      </c>
+      <c r="C84" t="s">
+        <v>124</v>
+      </c>
+      <c r="D84" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A85">
+        <v>6.7</v>
+      </c>
+      <c r="B85" t="s">
+        <v>42</v>
+      </c>
+      <c r="C85" t="s">
+        <v>125</v>
+      </c>
+      <c r="D85" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A86">
+        <v>6.8</v>
+      </c>
+      <c r="B86" t="s">
+        <v>42</v>
+      </c>
+      <c r="C86" t="s">
+        <v>126</v>
+      </c>
+      <c r="D86" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A87">
+        <v>6.9</v>
+      </c>
+      <c r="B87" t="s">
+        <v>42</v>
+      </c>
+      <c r="C87" t="s">
+        <v>127</v>
+      </c>
+      <c r="D87" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A88">
+        <v>6.1</v>
+      </c>
+      <c r="B88" t="s">
+        <v>42</v>
+      </c>
+      <c r="C88" t="s">
+        <v>128</v>
+      </c>
+      <c r="D88" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A89">
+        <v>6.11</v>
+      </c>
+      <c r="B89" t="s">
+        <v>42</v>
+      </c>
+      <c r="C89" t="s">
+        <v>129</v>
+      </c>
+      <c r="D89" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A90">
+        <v>6.12</v>
+      </c>
+      <c r="B90" t="s">
+        <v>42</v>
+      </c>
+      <c r="C90" t="s">
+        <v>130</v>
+      </c>
+      <c r="D90" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A91">
+        <v>6.13</v>
+      </c>
+      <c r="B91" t="s">
+        <v>42</v>
+      </c>
+      <c r="C91" t="s">
+        <v>131</v>
+      </c>
+      <c r="D91" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A92">
+        <v>6.14</v>
+      </c>
+      <c r="B92" t="s">
+        <v>42</v>
+      </c>
+      <c r="C92" t="s">
+        <v>132</v>
+      </c>
+      <c r="D92" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A93">
+        <v>6.15</v>
+      </c>
+      <c r="B93" t="s">
+        <v>42</v>
+      </c>
+      <c r="C93" t="s">
+        <v>133</v>
+      </c>
+      <c r="D93" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A94">
+        <v>6.16</v>
+      </c>
+      <c r="B94" t="s">
+        <v>42</v>
+      </c>
+      <c r="C94" t="s">
+        <v>134</v>
+      </c>
+      <c r="D94" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A95">
+        <v>6.17</v>
+      </c>
+      <c r="B95" t="s">
+        <v>42</v>
+      </c>
+      <c r="C95" t="s">
+        <v>135</v>
+      </c>
+      <c r="D95" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A96">
+        <v>6.18</v>
+      </c>
+      <c r="B96" t="s">
+        <v>42</v>
+      </c>
+      <c r="C96" t="s">
+        <v>136</v>
+      </c>
+      <c r="D96" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A97">
+        <v>6.19</v>
+      </c>
+      <c r="B97" t="s">
+        <v>42</v>
+      </c>
+      <c r="C97" t="s">
+        <v>137</v>
+      </c>
+      <c r="D97" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A98">
+        <v>6.2</v>
+      </c>
+      <c r="B98" t="s">
+        <v>42</v>
+      </c>
+      <c r="C98" t="s">
+        <v>138</v>
+      </c>
+      <c r="D98" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A99">
+        <v>6.21</v>
+      </c>
+      <c r="B99" t="s">
+        <v>42</v>
+      </c>
+      <c r="C99" t="s">
+        <v>139</v>
+      </c>
+      <c r="D99" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A100">
+        <v>6.22</v>
+      </c>
+      <c r="B100" t="s">
+        <v>42</v>
+      </c>
+      <c r="C100" t="s">
+        <v>140</v>
+      </c>
+      <c r="D100" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A101">
+        <v>6.23</v>
+      </c>
+      <c r="B101" t="s">
+        <v>42</v>
+      </c>
+      <c r="C101" t="s">
+        <v>141</v>
+      </c>
+      <c r="D101" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A102">
+        <v>6.24</v>
+      </c>
+      <c r="B102" t="s">
+        <v>42</v>
+      </c>
+      <c r="C102" t="s">
+        <v>142</v>
+      </c>
+      <c r="D102" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A103">
+        <v>7.1</v>
+      </c>
+      <c r="B103" t="s">
+        <v>43</v>
+      </c>
+      <c r="C103" t="s">
+        <v>21</v>
+      </c>
+      <c r="D103" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A104">
+        <v>7.2</v>
+      </c>
+      <c r="B104" t="s">
+        <v>43</v>
+      </c>
+      <c r="C104" t="s">
+        <v>143</v>
+      </c>
+      <c r="D104" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A105">
+        <v>7.3</v>
+      </c>
+      <c r="B105" t="s">
+        <v>43</v>
+      </c>
+      <c r="C105" t="s">
+        <v>144</v>
+      </c>
+      <c r="D105" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A106">
+        <v>7.4</v>
+      </c>
+      <c r="B106" t="s">
+        <v>43</v>
+      </c>
+      <c r="C106" t="s">
+        <v>145</v>
+      </c>
+      <c r="D106" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A107">
+        <v>7.5</v>
+      </c>
+      <c r="B107" t="s">
+        <v>43</v>
+      </c>
+      <c r="C107" t="s">
+        <v>146</v>
+      </c>
+      <c r="D107" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A108">
+        <v>7.6</v>
+      </c>
+      <c r="B108" t="s">
+        <v>43</v>
+      </c>
+      <c r="C108" t="s">
+        <v>147</v>
+      </c>
+      <c r="D108" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A109">
+        <v>7.7</v>
+      </c>
+      <c r="B109" t="s">
+        <v>43</v>
+      </c>
+      <c r="C109" t="s">
+        <v>148</v>
+      </c>
+      <c r="D109" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A110">
+        <v>7.8</v>
+      </c>
+      <c r="B110" t="s">
+        <v>43</v>
+      </c>
+      <c r="C110" t="s">
+        <v>149</v>
+      </c>
+      <c r="D110" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A111">
+        <v>7.9</v>
+      </c>
+      <c r="B111" t="s">
+        <v>43</v>
+      </c>
+      <c r="C111" t="s">
+        <v>150</v>
+      </c>
+      <c r="D111" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A112">
+        <v>7.1</v>
+      </c>
+      <c r="B112" t="s">
+        <v>43</v>
+      </c>
+      <c r="C112" t="s">
+        <v>151</v>
+      </c>
+      <c r="D112" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A113">
+        <v>7.11</v>
+      </c>
+      <c r="B113" t="s">
+        <v>43</v>
+      </c>
+      <c r="C113" t="s">
+        <v>152</v>
+      </c>
+      <c r="D113" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A114">
+        <v>7.12</v>
+      </c>
+      <c r="B114" t="s">
+        <v>43</v>
+      </c>
+      <c r="C114" t="s">
+        <v>153</v>
+      </c>
+      <c r="D114" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A115">
+        <v>7.13</v>
+      </c>
+      <c r="B115" t="s">
+        <v>43</v>
+      </c>
+      <c r="C115" t="s">
+        <v>154</v>
+      </c>
+      <c r="D115" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A116">
+        <v>8.1</v>
+      </c>
+      <c r="B116" t="s">
+        <v>44</v>
+      </c>
+      <c r="C116" t="s">
+        <v>18</v>
+      </c>
+      <c r="D116" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A117">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="B117" t="s">
+        <v>44</v>
+      </c>
+      <c r="C117" t="s">
+        <v>24</v>
+      </c>
+      <c r="D117" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A118">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="B118" t="s">
+        <v>44</v>
+      </c>
+      <c r="C118" t="s">
+        <v>19</v>
+      </c>
+      <c r="D118" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A119">
+        <v>8.4</v>
+      </c>
+      <c r="B119" t="s">
+        <v>44</v>
+      </c>
+      <c r="C119" t="s">
+        <v>20</v>
+      </c>
+      <c r="D119" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A120">
+        <v>8.5</v>
+      </c>
+      <c r="B120" t="s">
+        <v>44</v>
+      </c>
+      <c r="C120" t="s">
+        <v>15</v>
+      </c>
+      <c r="D120" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A121">
+        <v>9.1</v>
+      </c>
+      <c r="B121" t="s">
+        <v>17</v>
+      </c>
+      <c r="C121" t="s">
+        <v>11</v>
+      </c>
+      <c r="D121" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A122">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="B122" t="s">
+        <v>17</v>
+      </c>
+      <c r="C122" t="s">
+        <v>12</v>
+      </c>
+      <c r="D122" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A123">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="B123" t="s">
+        <v>17</v>
+      </c>
+      <c r="C123" t="s">
+        <v>13</v>
+      </c>
+      <c r="D123" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A124">
+        <v>9.4</v>
+      </c>
+      <c r="B124" t="s">
+        <v>17</v>
+      </c>
+      <c r="C124" t="s">
+        <v>14</v>
+      </c>
+      <c r="D124" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A125">
+        <v>9.5</v>
+      </c>
+      <c r="B125" t="s">
+        <v>17</v>
+      </c>
+      <c r="C125" t="s">
+        <v>16</v>
+      </c>
+      <c r="D125" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{451F0EA8-82C5-4B7F-9BA5-DBFED7B80306}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -951,13 +3100,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -965,10 +3114,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -976,10 +3125,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -987,10 +3136,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
@@ -998,10 +3147,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
@@ -1009,10 +3158,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>